<commit_message>
fix Tran Duc Trung link
</commit_message>
<xml_diff>
--- a/assignment1/response.xlsx
+++ b/assignment1/response.xlsx
@@ -2533,7 +2533,7 @@
     <t xml:space="preserve">Mã nguồn:
 https://github.com/niits/INT3411
 Dữ liệu:
-https://drive.google.com/file/d/1nt9XYeYhZFdeyLhMSVyL4wgmU1KY2zbd/view?usp=sharing</t>
+https://drive.google.com/file/d/1nt9XYeYhZFdeyLhMSVyL4wgmU1KY2zbd/view?usp=sharing </t>
   </si>
   <si>
     <t xml:space="preserve">2 Tháng tư 2020  10:13 AM</t>
@@ -3433,8 +3433,8 @@
   </sheetPr>
   <dimension ref="A1:K287"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F149" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K169" activeCellId="0" sqref="K169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8328,7 +8328,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="97.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="s">
         <v>94</v>
       </c>

</xml_diff>

<commit_message>
fix link Duong Thu Ha
</commit_message>
<xml_diff>
--- a/assignment1/response.xlsx
+++ b/assignment1/response.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2584" uniqueCount="1045">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2584" uniqueCount="1046">
   <si>
     <t xml:space="preserve">Họ và đệm</t>
   </si>
@@ -2178,6 +2178,10 @@
   </si>
   <si>
     <t xml:space="preserve">30 Tháng ba 2020  10:32 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code: https://github.com/duongghaa/speechProcessing/tree/master/Tuan1_thudulieu
+Data: https://drive.google.com/file/d/179rdOz4fulFvVCyDV3w_fub70M7YyQYM/view?usp=sharing </t>
   </si>
   <si>
     <t xml:space="preserve">30 Tháng ba 2020  10:52 PM</t>
@@ -3433,8 +3437,8 @@
   </sheetPr>
   <dimension ref="A1:K287"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F149" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K169" activeCellId="0" sqref="K169"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F222" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K238" activeCellId="0" sqref="K238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7342,7 +7346,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="61.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
         <v>33</v>
       </c>
@@ -7368,7 +7372,7 @@
         <v>18</v>
       </c>
       <c r="K135" s="1" t="s">
-        <v>666</v>
+        <v>689</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="115.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7385,19 +7389,19 @@
         <v>14</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="H136" s="1" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="I136" s="1" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="J136" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K136" s="1" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7414,19 +7418,19 @@
         <v>14</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="H137" s="1" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="I137" s="1" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="J137" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K137" s="1" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7443,19 +7447,19 @@
         <v>14</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="H138" s="1" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="I138" s="1" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="J138" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K138" s="1" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7472,19 +7476,19 @@
         <v>14</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="H139" s="1" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="I139" s="1" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="J139" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K139" s="1" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7501,19 +7505,19 @@
         <v>14</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="H140" s="1" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="I140" s="1" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="J140" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K140" s="1" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7530,13 +7534,13 @@
         <v>14</v>
       </c>
       <c r="G141" s="1" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="H141" s="1" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="I141" s="1" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="J141" s="1" t="s">
         <v>18</v>
@@ -7562,16 +7566,16 @@
         <v>653</v>
       </c>
       <c r="H142" s="1" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="I142" s="1" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="J142" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K142" s="1" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7588,10 +7592,10 @@
         <v>14</v>
       </c>
       <c r="G143" s="1" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="H143" s="1" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="I143" s="1" t="s">
         <v>603</v>
@@ -7600,7 +7604,7 @@
         <v>18</v>
       </c>
       <c r="K143" s="1" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7617,19 +7621,19 @@
         <v>14</v>
       </c>
       <c r="G144" s="1" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="H144" s="1" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="I144" s="1" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="J144" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K144" s="1" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7646,13 +7650,13 @@
         <v>14</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="H145" s="1" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="I145" s="1" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="J145" s="1" t="s">
         <v>18</v>
@@ -7675,19 +7679,19 @@
         <v>14</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="H146" s="1" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="I146" s="1" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="J146" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K146" s="1" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7704,13 +7708,13 @@
         <v>14</v>
       </c>
       <c r="G147" s="1" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="H147" s="1" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="I147" s="1" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="J147" s="1" t="s">
         <v>18</v>
@@ -7733,10 +7737,10 @@
         <v>14</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="H148" s="1" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="I148" s="1" t="s">
         <v>515</v>
@@ -7745,7 +7749,7 @@
         <v>18</v>
       </c>
       <c r="K148" s="1" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7762,19 +7766,19 @@
         <v>14</v>
       </c>
       <c r="G149" s="1" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="H149" s="1" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="I149" s="1" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="J149" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K149" s="1" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7791,48 +7795,48 @@
         <v>14</v>
       </c>
       <c r="G150" s="1" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="H150" s="1" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="I150" s="1" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="J150" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K150" s="1" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="1" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="F151" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G151" s="1" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="H151" s="1" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="I151" s="1" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="J151" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K151" s="1" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7849,19 +7853,19 @@
         <v>14</v>
       </c>
       <c r="G152" s="1" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="H152" s="1" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="I152" s="1" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="J152" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K152" s="1" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7878,10 +7882,10 @@
         <v>14</v>
       </c>
       <c r="G153" s="1" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="H153" s="1" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="I153" s="1" t="s">
         <v>576</v>
@@ -7907,13 +7911,13 @@
         <v>14</v>
       </c>
       <c r="G154" s="1" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="H154" s="1" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="I154" s="1" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="J154" s="1" t="s">
         <v>18</v>
@@ -7936,10 +7940,10 @@
         <v>14</v>
       </c>
       <c r="G155" s="1" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="H155" s="1" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="I155" s="1" t="s">
         <v>576</v>
@@ -7965,13 +7969,13 @@
         <v>14</v>
       </c>
       <c r="G156" s="1" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="H156" s="1" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="I156" s="1" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="J156" s="1" t="s">
         <v>18</v>
@@ -7994,19 +7998,19 @@
         <v>14</v>
       </c>
       <c r="G157" s="1" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="H157" s="1" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="I157" s="1" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="J157" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K157" s="1" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8023,19 +8027,19 @@
         <v>14</v>
       </c>
       <c r="G158" s="1" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="H158" s="1" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="I158" s="1" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="J158" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K158" s="1" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8052,10 +8056,10 @@
         <v>14</v>
       </c>
       <c r="G159" s="1" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="H159" s="1" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="I159" s="1" t="s">
         <v>651</v>
@@ -8064,7 +8068,7 @@
         <v>18</v>
       </c>
       <c r="K159" s="1" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8081,19 +8085,19 @@
         <v>14</v>
       </c>
       <c r="G160" s="1" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="H160" s="1" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="I160" s="1" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="J160" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K160" s="1" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8110,19 +8114,19 @@
         <v>14</v>
       </c>
       <c r="G161" s="1" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="H161" s="1" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="I161" s="1" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="J161" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K161" s="1" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8139,10 +8143,10 @@
         <v>14</v>
       </c>
       <c r="G162" s="1" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="H162" s="1" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="I162" s="1" t="s">
         <v>444</v>
@@ -8151,7 +8155,7 @@
         <v>18</v>
       </c>
       <c r="K162" s="1" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8168,13 +8172,13 @@
         <v>14</v>
       </c>
       <c r="G163" s="1" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="H163" s="1" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="I163" s="1" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="J163" s="1" t="s">
         <v>18</v>
@@ -8197,19 +8201,19 @@
         <v>14</v>
       </c>
       <c r="G164" s="1" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="H164" s="1" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="I164" s="1" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="J164" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K164" s="1" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8226,19 +8230,19 @@
         <v>14</v>
       </c>
       <c r="G165" s="1" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="H165" s="1" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="I165" s="1" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="J165" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K165" s="1" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8255,19 +8259,19 @@
         <v>14</v>
       </c>
       <c r="G166" s="1" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="H166" s="1" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="I166" s="1" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="J166" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K166" s="1" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8284,19 +8288,19 @@
         <v>14</v>
       </c>
       <c r="G167" s="1" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="H167" s="1" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="I167" s="1" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="J167" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K167" s="1" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8313,19 +8317,19 @@
         <v>14</v>
       </c>
       <c r="G168" s="1" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="H168" s="1" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="I168" s="1" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="J168" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K168" s="1" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="97.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8342,10 +8346,10 @@
         <v>14</v>
       </c>
       <c r="G169" s="1" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="H169" s="1" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="I169" s="1" t="s">
         <v>571</v>
@@ -8354,7 +8358,7 @@
         <v>18</v>
       </c>
       <c r="K169" s="1" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8371,19 +8375,19 @@
         <v>14</v>
       </c>
       <c r="G170" s="1" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="H170" s="1" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="I170" s="1" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="J170" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K170" s="1" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8400,19 +8404,19 @@
         <v>14</v>
       </c>
       <c r="G171" s="1" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="H171" s="1" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="I171" s="1" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="J171" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K171" s="1" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8429,19 +8433,19 @@
         <v>14</v>
       </c>
       <c r="G172" s="1" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="H172" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="I172" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="J172" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K172" s="1" t="s">
         <v>802</v>
-      </c>
-      <c r="I172" s="1" t="s">
-        <v>803</v>
-      </c>
-      <c r="J172" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K172" s="1" t="s">
-        <v>801</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8458,13 +8462,13 @@
         <v>14</v>
       </c>
       <c r="G173" s="1" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="H173" s="1" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="I173" s="1" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="J173" s="1" t="s">
         <v>18</v>
@@ -8487,19 +8491,19 @@
         <v>14</v>
       </c>
       <c r="G174" s="1" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="H174" s="1" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="I174" s="1" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="J174" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K174" s="1" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8516,19 +8520,19 @@
         <v>14</v>
       </c>
       <c r="G175" s="1" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="H175" s="1" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="I175" s="1" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="J175" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K175" s="1" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8545,19 +8549,19 @@
         <v>14</v>
       </c>
       <c r="G176" s="1" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="H176" s="1" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="I176" s="1" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="J176" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K176" s="1" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8574,19 +8578,19 @@
         <v>14</v>
       </c>
       <c r="G177" s="1" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="H177" s="1" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="I177" s="1" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="J177" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K177" s="1" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8603,39 +8607,39 @@
         <v>14</v>
       </c>
       <c r="G178" s="1" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="H178" s="1" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="I178" s="1" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="J178" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K178" s="1" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="1" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="F179" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G179" s="1" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="H179" s="1" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="I179" s="1" t="s">
         <v>651</v>
@@ -8644,7 +8648,7 @@
         <v>18</v>
       </c>
       <c r="K179" s="1" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8661,10 +8665,10 @@
         <v>14</v>
       </c>
       <c r="G180" s="1" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="H180" s="1" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="I180" s="1" t="s">
         <v>497</v>
@@ -8673,7 +8677,7 @@
         <v>18</v>
       </c>
       <c r="K180" s="1" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8690,19 +8694,19 @@
         <v>14</v>
       </c>
       <c r="G181" s="1" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="H181" s="1" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="I181" s="1" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="J181" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K181" s="1" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8719,19 +8723,19 @@
         <v>14</v>
       </c>
       <c r="G182" s="1" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="H182" s="1" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="I182" s="1" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="J182" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K182" s="1" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8748,19 +8752,19 @@
         <v>14</v>
       </c>
       <c r="G183" s="1" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="H183" s="1" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="I183" s="1" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="J183" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K183" s="1" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8777,13 +8781,13 @@
         <v>14</v>
       </c>
       <c r="G184" s="1" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="H184" s="1" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="I184" s="1" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="J184" s="1" t="s">
         <v>18</v>
@@ -8806,13 +8810,13 @@
         <v>14</v>
       </c>
       <c r="G185" s="1" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="H185" s="1" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="I185" s="1" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="J185" s="1" t="s">
         <v>18</v>
@@ -8835,19 +8839,19 @@
         <v>14</v>
       </c>
       <c r="G186" s="1" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="H186" s="1" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="I186" s="1" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="J186" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K186" s="1" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8864,19 +8868,19 @@
         <v>14</v>
       </c>
       <c r="G187" s="1" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="H187" s="1" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="I187" s="1" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J187" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K187" s="1" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8893,19 +8897,19 @@
         <v>14</v>
       </c>
       <c r="G188" s="1" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="H188" s="1" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="I188" s="1" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="J188" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K188" s="1" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8922,19 +8926,19 @@
         <v>14</v>
       </c>
       <c r="G189" s="1" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="H189" s="1" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="I189" s="1" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="J189" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K189" s="1" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8951,19 +8955,19 @@
         <v>14</v>
       </c>
       <c r="G190" s="1" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="H190" s="1" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="I190" s="1" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="J190" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K190" s="1" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8980,13 +8984,13 @@
         <v>14</v>
       </c>
       <c r="G191" s="1" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="H191" s="1" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="I191" s="1" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="J191" s="1" t="s">
         <v>18</v>
@@ -9009,13 +9013,13 @@
         <v>14</v>
       </c>
       <c r="G192" s="1" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="H192" s="1" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="I192" s="1" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="J192" s="1" t="s">
         <v>18</v>
@@ -9038,13 +9042,13 @@
         <v>14</v>
       </c>
       <c r="G193" s="1" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="H193" s="1" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="I193" s="1" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="J193" s="1" t="s">
         <v>18</v>
@@ -9067,19 +9071,19 @@
         <v>14</v>
       </c>
       <c r="G194" s="1" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="H194" s="1" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="I194" s="1" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="J194" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K194" s="1" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9099,7 +9103,7 @@
         <v>622</v>
       </c>
       <c r="H195" s="1" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="I195" s="1" t="s">
         <v>330</v>
@@ -9108,7 +9112,7 @@
         <v>18</v>
       </c>
       <c r="K195" s="1" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9125,19 +9129,19 @@
         <v>14</v>
       </c>
       <c r="G196" s="1" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="H196" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="I196" s="1" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="J196" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K196" s="1" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9154,19 +9158,19 @@
         <v>14</v>
       </c>
       <c r="G197" s="1" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="H197" s="1" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="I197" s="1" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="J197" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K197" s="1" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9183,48 +9187,48 @@
         <v>14</v>
       </c>
       <c r="G198" s="1" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="H198" s="1" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="I198" s="1" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="J198" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K198" s="1" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="1" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>352</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="F199" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G199" s="1" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="H199" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="I199" s="1" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="J199" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K199" s="1" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9241,48 +9245,48 @@
         <v>14</v>
       </c>
       <c r="G200" s="1" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="H200" s="1" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="I200" s="1" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="J200" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K200" s="1" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="1" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="F201" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G201" s="1" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="H201" s="1" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="I201" s="1" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="J201" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K201" s="1" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9299,13 +9303,13 @@
         <v>14</v>
       </c>
       <c r="G202" s="1" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="H202" s="1" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="I202" s="1" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="J202" s="1" t="s">
         <v>18</v>
@@ -9325,19 +9329,19 @@
         <v>14</v>
       </c>
       <c r="G203" s="1" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="H203" s="1" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="I203" s="1" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="J203" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K203" s="1" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9354,10 +9358,10 @@
         <v>14</v>
       </c>
       <c r="G204" s="1" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="H204" s="1" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="I204" s="1" t="s">
         <v>626</v>
@@ -9383,10 +9387,10 @@
         <v>14</v>
       </c>
       <c r="G205" s="1" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="H205" s="1" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="I205" s="1" t="s">
         <v>515</v>
@@ -9412,13 +9416,13 @@
         <v>14</v>
       </c>
       <c r="G206" s="1" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="H206" s="1" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="I206" s="1" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="J206" s="1" t="s">
         <v>18</v>
@@ -9441,13 +9445,13 @@
         <v>14</v>
       </c>
       <c r="G207" s="1" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="H207" s="1" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="I207" s="1" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="J207" s="1" t="s">
         <v>18</v>
@@ -9470,19 +9474,19 @@
         <v>14</v>
       </c>
       <c r="G208" s="1" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="H208" s="1" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="I208" s="1" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="J208" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K208" s="1" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9499,10 +9503,10 @@
         <v>14</v>
       </c>
       <c r="G209" s="1" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="H209" s="1" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="I209" s="1" t="s">
         <v>497</v>
@@ -9528,10 +9532,10 @@
         <v>14</v>
       </c>
       <c r="G210" s="1" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="H210" s="1" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="I210" s="1" t="s">
         <v>497</v>
@@ -9540,7 +9544,7 @@
         <v>18</v>
       </c>
       <c r="K210" s="1" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9557,10 +9561,10 @@
         <v>14</v>
       </c>
       <c r="G211" s="1" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="H211" s="1" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="I211" s="1" t="s">
         <v>626</v>
@@ -9586,10 +9590,10 @@
         <v>14</v>
       </c>
       <c r="G212" s="1" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="H212" s="1" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="I212" s="1" t="s">
         <v>497</v>
@@ -9598,7 +9602,7 @@
         <v>18</v>
       </c>
       <c r="K212" s="1" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9615,19 +9619,19 @@
         <v>14</v>
       </c>
       <c r="G213" s="1" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="H213" s="1" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="I213" s="1" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="J213" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K213" s="1" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9644,13 +9648,13 @@
         <v>14</v>
       </c>
       <c r="G214" s="1" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="H214" s="1" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="I214" s="1" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="J214" s="1" t="s">
         <v>18</v>
@@ -9673,10 +9677,10 @@
         <v>14</v>
       </c>
       <c r="G215" s="1" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="H215" s="1" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="I215" s="1" t="s">
         <v>644</v>
@@ -9685,7 +9689,7 @@
         <v>18</v>
       </c>
       <c r="K215" s="1" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9702,13 +9706,13 @@
         <v>14</v>
       </c>
       <c r="G216" s="1" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="H216" s="1" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="I216" s="1" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="J216" s="1" t="s">
         <v>18</v>
@@ -9731,19 +9735,19 @@
         <v>14</v>
       </c>
       <c r="G217" s="1" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="H217" s="1" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="I217" s="1" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="J217" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K217" s="1" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9760,10 +9764,10 @@
         <v>14</v>
       </c>
       <c r="G218" s="1" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="H218" s="1" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="I218" s="1" t="s">
         <v>569</v>
@@ -9772,7 +9776,7 @@
         <v>18</v>
       </c>
       <c r="K218" s="1" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9789,10 +9793,10 @@
         <v>14</v>
       </c>
       <c r="G219" s="1" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="H219" s="1" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="I219" s="1" t="s">
         <v>497</v>
@@ -9801,7 +9805,7 @@
         <v>18</v>
       </c>
       <c r="K219" s="1" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9818,19 +9822,19 @@
         <v>14</v>
       </c>
       <c r="G220" s="1" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="H220" s="1" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="I220" s="1" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="J220" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K220" s="1" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9847,19 +9851,19 @@
         <v>14</v>
       </c>
       <c r="G221" s="1" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="H221" s="1" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="I221" s="1" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="J221" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K221" s="1" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9876,19 +9880,19 @@
         <v>14</v>
       </c>
       <c r="G222" s="1" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="H222" s="1" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="I222" s="1" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="J222" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K222" s="1" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9911,13 +9915,13 @@
         <v>455</v>
       </c>
       <c r="I223" s="1" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="J223" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K223" s="1" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9934,19 +9938,19 @@
         <v>14</v>
       </c>
       <c r="G224" s="1" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="H224" s="1" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="I224" s="1" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="J224" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K224" s="1" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9963,10 +9967,10 @@
         <v>14</v>
       </c>
       <c r="G225" s="1" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="H225" s="1" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="I225" s="1" t="s">
         <v>603</v>
@@ -9992,13 +9996,13 @@
         <v>14</v>
       </c>
       <c r="G226" s="1" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="H226" s="1" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="I226" s="1" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="J226" s="1" t="s">
         <v>18</v>
@@ -10021,19 +10025,19 @@
         <v>14</v>
       </c>
       <c r="G227" s="1" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="H227" s="1" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="I227" s="1" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="J227" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K227" s="1" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10050,19 +10054,19 @@
         <v>14</v>
       </c>
       <c r="G228" s="1" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="H228" s="1" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="I228" s="1" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="J228" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K228" s="1" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10079,10 +10083,10 @@
         <v>14</v>
       </c>
       <c r="G229" s="1" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="H229" s="1" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="I229" s="1" t="s">
         <v>571</v>
@@ -10091,7 +10095,7 @@
         <v>18</v>
       </c>
       <c r="K229" s="1" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10108,19 +10112,19 @@
         <v>14</v>
       </c>
       <c r="G230" s="1" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="H230" s="1" t="s">
+        <v>950</v>
+      </c>
+      <c r="I230" s="1" t="s">
+        <v>903</v>
+      </c>
+      <c r="J230" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K230" s="1" t="s">
         <v>949</v>
-      </c>
-      <c r="I230" s="1" t="s">
-        <v>902</v>
-      </c>
-      <c r="J230" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K230" s="1" t="s">
-        <v>948</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10137,19 +10141,19 @@
         <v>14</v>
       </c>
       <c r="G231" s="1" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="H231" s="1" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="I231" s="1" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="J231" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K231" s="1" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10166,10 +10170,10 @@
         <v>14</v>
       </c>
       <c r="G232" s="1" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="H232" s="1" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="I232" s="1" t="s">
         <v>651</v>
@@ -10178,7 +10182,7 @@
         <v>18</v>
       </c>
       <c r="K232" s="1" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10195,77 +10199,77 @@
         <v>14</v>
       </c>
       <c r="G233" s="1" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="H233" s="1" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="I233" s="1" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="J233" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K233" s="1" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="1" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="B234" s="1" t="s">
         <v>319</v>
       </c>
       <c r="E234" s="1" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="F234" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G234" s="1" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="H234" s="1" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="I234" s="1" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="J234" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K234" s="1" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="1" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="B235" s="1" t="s">
         <v>319</v>
       </c>
       <c r="E235" s="1" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="F235" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G235" s="1" t="s">
+        <v>966</v>
+      </c>
+      <c r="H235" s="1" t="s">
+        <v>967</v>
+      </c>
+      <c r="I235" s="1" t="s">
+        <v>968</v>
+      </c>
+      <c r="J235" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K235" s="1" t="s">
         <v>965</v>
-      </c>
-      <c r="H235" s="1" t="s">
-        <v>966</v>
-      </c>
-      <c r="I235" s="1" t="s">
-        <v>967</v>
-      </c>
-      <c r="J235" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K235" s="1" t="s">
-        <v>964</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10282,10 +10286,10 @@
         <v>14</v>
       </c>
       <c r="G236" s="1" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="H236" s="1" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="I236" s="1" t="s">
         <v>449</v>
@@ -10294,10 +10298,10 @@
         <v>18</v>
       </c>
       <c r="K236" s="1" t="s">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="237" customFormat="false" ht="61.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="1" t="s">
         <v>33</v>
       </c>
@@ -10311,10 +10315,10 @@
         <v>14</v>
       </c>
       <c r="G237" s="1" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="H237" s="1" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="I237" s="1" t="s">
         <v>651</v>
@@ -10323,36 +10327,36 @@
         <v>18</v>
       </c>
       <c r="K237" s="1" t="s">
-        <v>761</v>
+        <v>689</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="1" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="B238" s="1" t="s">
         <v>352</v>
       </c>
       <c r="E238" s="1" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="F238" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G238" s="1" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="H238" s="1" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="I238" s="1" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="J238" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K238" s="1" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10372,16 +10376,16 @@
         <v>500</v>
       </c>
       <c r="H239" s="1" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="I239" s="1" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="J239" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K239" s="1" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10398,19 +10402,19 @@
         <v>14</v>
       </c>
       <c r="G240" s="1" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="H240" s="1" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="I240" s="1" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="J240" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K240" s="1" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10427,10 +10431,10 @@
         <v>14</v>
       </c>
       <c r="G241" s="1" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="H241" s="1" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="I241" s="1" t="s">
         <v>576</v>
@@ -10439,7 +10443,7 @@
         <v>18</v>
       </c>
       <c r="K241" s="1" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10456,10 +10460,10 @@
         <v>14</v>
       </c>
       <c r="G242" s="1" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="H242" s="1" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="I242" s="1" t="s">
         <v>626</v>
@@ -10485,19 +10489,19 @@
         <v>14</v>
       </c>
       <c r="G243" s="1" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="H243" s="1" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="I243" s="1" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="J243" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K243" s="1" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10508,25 +10512,25 @@
         <v>288</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="F244" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G244" s="1" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="H244" s="1" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="I244" s="1" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="J244" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K244" s="1" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10537,25 +10541,25 @@
         <v>288</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="F245" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G245" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="H245" s="1" t="s">
+        <v>993</v>
+      </c>
+      <c r="I245" s="1" t="s">
+        <v>968</v>
+      </c>
+      <c r="J245" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K245" s="1" t="s">
         <v>991</v>
-      </c>
-      <c r="H245" s="1" t="s">
-        <v>992</v>
-      </c>
-      <c r="I245" s="1" t="s">
-        <v>967</v>
-      </c>
-      <c r="J245" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K245" s="1" t="s">
-        <v>990</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10572,10 +10576,10 @@
         <v>14</v>
       </c>
       <c r="G246" s="1" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="H246" s="1" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="I246" s="1" t="s">
         <v>576</v>
@@ -10595,13 +10599,13 @@
         <v>217</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="F247" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G247" s="1" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="H247" s="1" t="s">
         <v>503</v>
@@ -10618,19 +10622,19 @@
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="1" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="E248" s="1" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="F248" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G248" s="1" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="H248" s="1" t="s">
         <v>503</v>
@@ -10653,13 +10657,13 @@
         <v>126</v>
       </c>
       <c r="E249" s="1" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="F249" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G249" s="1" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="H249" s="1" t="s">
         <v>503</v>
@@ -10685,10 +10689,10 @@
         <v>76</v>
       </c>
       <c r="F250" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G250" s="1" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="H250" s="1" t="s">
         <v>503</v>
@@ -10714,10 +10718,10 @@
         <v>471</v>
       </c>
       <c r="F251" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G251" s="1" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="H251" s="1" t="s">
         <v>503</v>
@@ -10743,10 +10747,10 @@
         <v>108</v>
       </c>
       <c r="F252" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G252" s="1" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="H252" s="1" t="s">
         <v>503</v>
@@ -10763,19 +10767,19 @@
     </row>
     <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="1" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="B253" s="1" t="s">
         <v>584</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="F253" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G253" s="1" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="H253" s="1" t="s">
         <v>503</v>
@@ -10801,10 +10805,10 @@
         <v>513</v>
       </c>
       <c r="F254" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G254" s="1" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="H254" s="1" t="s">
         <v>503</v>
@@ -10830,10 +10834,10 @@
         <v>683</v>
       </c>
       <c r="F255" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G255" s="1" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="H255" s="1" t="s">
         <v>503</v>
@@ -10859,10 +10863,10 @@
         <v>69</v>
       </c>
       <c r="F256" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G256" s="1" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="H256" s="1" t="s">
         <v>503</v>
@@ -10888,10 +10892,10 @@
         <v>540</v>
       </c>
       <c r="F257" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G257" s="1" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="H257" s="1" t="s">
         <v>503</v>
@@ -10917,10 +10921,10 @@
         <v>29</v>
       </c>
       <c r="F258" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G258" s="1" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="H258" s="1" t="s">
         <v>503</v>
@@ -10946,10 +10950,10 @@
         <v>13</v>
       </c>
       <c r="F259" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G259" s="1" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="H259" s="1" t="s">
         <v>503</v>
@@ -10966,19 +10970,19 @@
     </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="1" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="E260" s="1" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="F260" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G260" s="1" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="H260" s="1" t="s">
         <v>503</v>
@@ -11004,10 +11008,10 @@
         <v>237</v>
       </c>
       <c r="F261" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G261" s="1" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="H261" s="1" t="s">
         <v>503</v>
@@ -11033,10 +11037,10 @@
         <v>89</v>
       </c>
       <c r="F262" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G262" s="1" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="H262" s="1" t="s">
         <v>503</v>
@@ -11062,10 +11066,10 @@
         <v>585</v>
       </c>
       <c r="F263" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G263" s="1" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="H263" s="1" t="s">
         <v>503</v>
@@ -11091,10 +11095,10 @@
         <v>138</v>
       </c>
       <c r="F264" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G264" s="1" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="H264" s="1" t="s">
         <v>503</v>
@@ -11120,10 +11124,10 @@
         <v>283</v>
       </c>
       <c r="F265" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G265" s="1" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="H265" s="1" t="s">
         <v>503</v>
@@ -11149,10 +11153,10 @@
         <v>578</v>
       </c>
       <c r="F266" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G266" s="1" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="H266" s="1" t="s">
         <v>503</v>
@@ -11178,10 +11182,10 @@
         <v>218</v>
       </c>
       <c r="F267" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G267" s="1" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="H267" s="1" t="s">
         <v>503</v>
@@ -11207,10 +11211,10 @@
         <v>132</v>
       </c>
       <c r="F268" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G268" s="1" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="H268" s="1" t="s">
         <v>503</v>
@@ -11236,10 +11240,10 @@
         <v>155</v>
       </c>
       <c r="F269" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G269" s="1" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="H269" s="1" t="s">
         <v>503</v>
@@ -11265,10 +11269,10 @@
         <v>359</v>
       </c>
       <c r="F270" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G270" s="1" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="H270" s="1" t="s">
         <v>503</v>
@@ -11294,10 +11298,10 @@
         <v>167</v>
       </c>
       <c r="F271" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G271" s="1" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="H271" s="1" t="s">
         <v>503</v>
@@ -11323,10 +11327,10 @@
         <v>270</v>
       </c>
       <c r="F272" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G272" s="1" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="H272" s="1" t="s">
         <v>503</v>
@@ -11352,10 +11356,10 @@
         <v>441</v>
       </c>
       <c r="F273" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G273" s="1" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="H273" s="1" t="s">
         <v>503</v>
@@ -11381,10 +11385,10 @@
         <v>313</v>
       </c>
       <c r="F274" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G274" s="1" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="H274" s="1" t="s">
         <v>503</v>
@@ -11401,19 +11405,19 @@
     </row>
     <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="1" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="B275" s="1" t="s">
         <v>319</v>
       </c>
       <c r="E275" s="1" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="F275" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G275" s="1" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="H275" s="1" t="s">
         <v>503</v>
@@ -11439,10 +11443,10 @@
         <v>121</v>
       </c>
       <c r="F276" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G276" s="1" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="H276" s="1" t="s">
         <v>503</v>
@@ -11468,10 +11472,10 @@
         <v>365</v>
       </c>
       <c r="F277" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G277" s="1" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="H277" s="1" t="s">
         <v>503</v>
@@ -11497,10 +11501,10 @@
         <v>391</v>
       </c>
       <c r="F278" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G278" s="1" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="H278" s="1" t="s">
         <v>503</v>
@@ -11517,19 +11521,19 @@
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="1" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="B279" s="1" t="s">
         <v>126</v>
       </c>
       <c r="E279" s="1" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="F279" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G279" s="1" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="H279" s="1" t="s">
         <v>503</v>
@@ -11555,10 +11559,10 @@
         <v>398</v>
       </c>
       <c r="F280" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G280" s="1" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="H280" s="1" t="s">
         <v>503</v>
@@ -11584,10 +11588,10 @@
         <v>340</v>
       </c>
       <c r="F281" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G281" s="1" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="H281" s="1" t="s">
         <v>503</v>
@@ -11613,10 +11617,10 @@
         <v>42</v>
       </c>
       <c r="F282" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G282" s="1" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="H282" s="1" t="s">
         <v>503</v>
@@ -11642,10 +11646,10 @@
         <v>307</v>
       </c>
       <c r="F283" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G283" s="1" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="H283" s="1" t="s">
         <v>503</v>
@@ -11671,10 +11675,10 @@
         <v>256</v>
       </c>
       <c r="F284" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G284" s="1" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="H284" s="1" t="s">
         <v>503</v>
@@ -11700,10 +11704,10 @@
         <v>289</v>
       </c>
       <c r="F285" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G285" s="1" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="H285" s="1" t="s">
         <v>503</v>
@@ -11726,13 +11730,13 @@
         <v>288</v>
       </c>
       <c r="E286" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="F286" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G286" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="H286" s="1" t="s">
         <v>503</v>
@@ -11758,10 +11762,10 @@
         <v>460</v>
       </c>
       <c r="F287" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="G287" s="1" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="H287" s="1" t="s">
         <v>503</v>

</xml_diff>